<commit_message>
ajeitando a funcionalidade extrair pdf
</commit_message>
<xml_diff>
--- a/Extracao-de-dados-pdf/docs/relatorio_cartao_sus.xlsx
+++ b/Extracao-de-dados-pdf/docs/relatorio_cartao_sus.xlsx
@@ -453,12 +453,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Isaac</t>
+          <t>Isaac Moreira</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Moreira</t>
+          <t>149.578.326-09</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -470,12 +470,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Igor</t>
+          <t>Igor Barros</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Barros</t>
+          <t>709.815.623-02</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -487,12 +487,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Vitória</t>
+          <t>Vitória Almeida</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Almeida</t>
+          <t>160.478.932-87</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -504,12 +504,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Amanda</t>
+          <t>Amanda Fernandes</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Fernandes</t>
+          <t>134.568.739-25</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -521,12 +521,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Lucas Pereira</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Pereira</t>
+          <t>268.235.174-60</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -538,12 +538,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Samuel</t>
+          <t>Samuel Costa</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Costa</t>
+          <t>874.123.756-50</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -555,12 +555,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Pedro</t>
+          <t>Pedro Almeida</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Almeida</t>
+          <t>194.854.362-91</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Santos</t>
+          <t>584.963.217-49</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -589,12 +589,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Beatriz</t>
+          <t>Beatriz Gomes</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Gomes</t>
+          <t>953.142.689-01</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -606,12 +606,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Leonardo</t>
+          <t>Leonardo Lima</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Lima</t>
+          <t>362.497.528-09</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -623,12 +623,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Gustavo</t>
+          <t>Gustavo Batista</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Batista</t>
+          <t>851.324.178-12</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -640,12 +640,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Daniel</t>
+          <t>Daniel Cunha</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Cunha</t>
+          <t>342.178.543-65</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -657,12 +657,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Matheus</t>
+          <t>Matheus Barros</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Barros</t>
+          <t>146.983.254-17</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -674,12 +674,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Rafael</t>
+          <t>Rafael Oliveira</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Oliveira</t>
+          <t>734.862.319-05</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -691,12 +691,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Renan</t>
+          <t>Renan Cardoso</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Cardoso</t>
+          <t>694.251.784-23</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -708,12 +708,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Diego</t>
+          <t>Diego Vieira</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Vieira</t>
+          <t>194.825.763-02</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -725,12 +725,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Bruno</t>
+          <t>Bruno Mendes</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Mendes</t>
+          <t>563.712.358-46</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -742,12 +742,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Thiago</t>
+          <t>Thiago Barbosa</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Barbosa</t>
+          <t>167.925.138-80</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -759,12 +759,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Henrique</t>
+          <t>Henrique Ferreira</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ferreira</t>
+          <t>643.187.925-48</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -776,12 +776,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Vinícius</t>
+          <t>Vinícius Oliveira</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Oliveira</t>
+          <t>694.871.352-10</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -793,12 +793,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>André</t>
+          <t>André Dias</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Dias</t>
+          <t>712.358.194-83</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -810,12 +810,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Nicole</t>
+          <t>Nicole Borges</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Borges</t>
+          <t>157.923.485-06</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -827,12 +827,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Lucas</t>
+          <t>Lucas Cavalcante</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Cavalcante</t>
+          <t>189.725.143-40</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -844,12 +844,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sérgio</t>
+          <t>Sérgio Correia</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Correia</t>
+          <t>583.491.763-90</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">

</xml_diff>